<commit_message>
update in GetListOfAllCandidatResumeRejected/ShortListed handler
</commit_message>
<xml_diff>
--- a/All_candidates.xlsx
+++ b/All_candidates.xlsx
@@ -382,10 +382,10 @@
       <c r="G2" t="str">
         <v>umesh@gmail.com</v>
       </c>
-      <c r="H2">
-        <v>16</v>
-      </c>
-      <c r="I2">
+      <c r="H2" t="str">
+        <v>16</v>
+      </c>
+      <c r="I2" t="str">
         <v>15</v>
       </c>
       <c r="J2" t="str">
@@ -420,10 +420,10 @@
       <c r="G3" t="str">
         <v>aditya@gmail.com</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="str">
         <v>5</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="str">
         <v>4</v>
       </c>
       <c r="J3" t="str">
@@ -458,10 +458,10 @@
       <c r="G4" t="str">
         <v>umesh@gmail.com</v>
       </c>
-      <c r="H4">
-        <v>16</v>
-      </c>
-      <c r="I4">
+      <c r="H4" t="str">
+        <v>16</v>
+      </c>
+      <c r="I4" t="str">
         <v>15</v>
       </c>
       <c r="J4" t="str">
@@ -496,10 +496,10 @@
       <c r="G5" t="str">
         <v>sathiya@gmail.com</v>
       </c>
-      <c r="H5">
-        <v>16</v>
-      </c>
-      <c r="I5">
+      <c r="H5" t="str">
+        <v>16</v>
+      </c>
+      <c r="I5" t="str">
         <v>15</v>
       </c>
       <c r="J5" t="str">
@@ -534,10 +534,10 @@
       <c r="G6" t="str">
         <v>yellaling@mai.com</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="str">
         <v>10</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="str">
         <v>9</v>
       </c>
       <c r="J6" t="str">
@@ -572,10 +572,10 @@
       <c r="G7" t="str">
         <v>shaik@gmail.com</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="str">
         <v>11</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="str">
         <v>10</v>
       </c>
       <c r="J7" t="str">
@@ -610,10 +610,10 @@
       <c r="G8" t="str">
         <v>saidameer@gmail.com</v>
       </c>
-      <c r="H8">
+      <c r="H8" t="str">
         <v>12</v>
       </c>
-      <c r="I8">
+      <c r="I8" t="str">
         <v>11</v>
       </c>
       <c r="J8" t="str">
@@ -648,10 +648,10 @@
       <c r="G9" t="str">
         <v>arpit@gmail.com</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="str">
         <v>13</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="str">
         <v>12</v>
       </c>
       <c r="J9" t="str">
@@ -686,10 +686,10 @@
       <c r="G10" t="str">
         <v>tishya@gmail.com</v>
       </c>
-      <c r="H10">
-        <v>16</v>
-      </c>
-      <c r="I10">
+      <c r="H10" t="str">
+        <v>16</v>
+      </c>
+      <c r="I10" t="str">
         <v>15</v>
       </c>
       <c r="J10" t="str">
@@ -724,10 +724,10 @@
       <c r="G11" t="str">
         <v>tishya@gmail.com</v>
       </c>
-      <c r="H11">
-        <v>16</v>
-      </c>
-      <c r="I11">
+      <c r="H11" t="str">
+        <v>16</v>
+      </c>
+      <c r="I11" t="str">
         <v>15</v>
       </c>
       <c r="J11" t="str">
@@ -762,10 +762,10 @@
       <c r="G12" t="str">
         <v>tishya@gmail.com</v>
       </c>
-      <c r="H12">
-        <v>16</v>
-      </c>
-      <c r="I12">
+      <c r="H12" t="str">
+        <v>16</v>
+      </c>
+      <c r="I12" t="str">
         <v>15</v>
       </c>
       <c r="J12" t="str">
@@ -800,10 +800,10 @@
       <c r="G13" t="str">
         <v>tishya@gmail.com</v>
       </c>
-      <c r="H13">
-        <v>16</v>
-      </c>
-      <c r="I13">
+      <c r="H13" t="str">
+        <v>16</v>
+      </c>
+      <c r="I13" t="str">
         <v>15</v>
       </c>
       <c r="J13" t="str">
@@ -838,10 +838,10 @@
       <c r="G14" t="str">
         <v>aman@gamil.com</v>
       </c>
-      <c r="H14">
+      <c r="H14" t="str">
         <v>10</v>
       </c>
-      <c r="I14">
+      <c r="I14" t="str">
         <v>10</v>
       </c>
       <c r="J14" t="str">
@@ -876,10 +876,10 @@
       <c r="G15" t="str">
         <v>tishya@gmail.com</v>
       </c>
-      <c r="H15">
-        <v>16</v>
-      </c>
-      <c r="I15">
+      <c r="H15" t="str">
+        <v>16</v>
+      </c>
+      <c r="I15" t="str">
         <v>15</v>
       </c>
       <c r="J15" t="str">
@@ -914,10 +914,10 @@
       <c r="G16" t="str">
         <v>roy1998@gmail.com</v>
       </c>
-      <c r="H16">
-        <v>16</v>
-      </c>
-      <c r="I16">
+      <c r="H16" t="str">
+        <v>16</v>
+      </c>
+      <c r="I16" t="str">
         <v>15</v>
       </c>
       <c r="J16" t="str">
@@ -952,10 +952,10 @@
       <c r="G17" t="str">
         <v>peter@gmail.com</v>
       </c>
-      <c r="H17">
-        <v>16</v>
-      </c>
-      <c r="I17">
+      <c r="H17" t="str">
+        <v>16</v>
+      </c>
+      <c r="I17" t="str">
         <v>15</v>
       </c>
       <c r="J17" t="str">
@@ -990,10 +990,10 @@
       <c r="G18" t="str">
         <v>surma@gmail.com</v>
       </c>
-      <c r="H18">
-        <v>16</v>
-      </c>
-      <c r="I18">
+      <c r="H18" t="str">
+        <v>16</v>
+      </c>
+      <c r="I18" t="str">
         <v>15</v>
       </c>
       <c r="J18" t="str">
@@ -1028,10 +1028,10 @@
       <c r="G19" t="str">
         <v>cleveland@gmail.com</v>
       </c>
-      <c r="H19">
-        <v>16</v>
-      </c>
-      <c r="I19">
+      <c r="H19" t="str">
+        <v>16</v>
+      </c>
+      <c r="I19" t="str">
         <v>15</v>
       </c>
       <c r="J19" t="str">
@@ -1049,39 +1049,115 @@
     </row>
     <row r="20">
       <c r="B20">
+        <v>318</v>
+      </c>
+      <c r="C20" t="str">
+        <v>2024-01-02</v>
+      </c>
+      <c r="D20" t="str">
+        <v>java</v>
+      </c>
+      <c r="E20" t="str">
+        <v>cleveland1</v>
+      </c>
+      <c r="F20" t="str">
+        <v>55667788</v>
+      </c>
+      <c r="G20" t="str">
+        <v>cleveland1@gmail.com</v>
+      </c>
+      <c r="H20" t="str">
+        <v>16</v>
+      </c>
+      <c r="I20" t="str">
+        <v>15</v>
+      </c>
+      <c r="J20" t="str">
+        <v>nasa corporation</v>
+      </c>
+      <c r="K20" t="str">
+        <v>3</v>
+      </c>
+      <c r="L20" t="str">
+        <v>upgraded for further interview level</v>
+      </c>
+      <c r="M20" t="str">
+        <v>shortlisted</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21">
+        <v>319</v>
+      </c>
+      <c r="C21" t="str">
+        <v>2024-01-02</v>
+      </c>
+      <c r="D21" t="str">
+        <v>java</v>
+      </c>
+      <c r="E21" t="str">
+        <v>surmak</v>
+      </c>
+      <c r="F21" t="str">
+        <v>55667788</v>
+      </c>
+      <c r="G21" t="str">
+        <v>surmka@gmail.com</v>
+      </c>
+      <c r="H21" t="str">
+        <v>16</v>
+      </c>
+      <c r="I21" t="str">
+        <v>15</v>
+      </c>
+      <c r="J21" t="str">
+        <v>umbrala corporation</v>
+      </c>
+      <c r="K21" t="str">
+        <v>3</v>
+      </c>
+      <c r="L21" t="str">
+        <v>upgraded for further interview level</v>
+      </c>
+      <c r="M21" t="str">
+        <v>shortlisted</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22">
         <v>320</v>
       </c>
-      <c r="C20" t="str">
+      <c r="C22" t="str">
         <v>2024-02-20</v>
       </c>
-      <c r="D20" t="str">
+      <c r="D22" t="str">
         <v>golang</v>
       </c>
-      <c r="E20" t="str">
+      <c r="E22" t="str">
         <v>harsh</v>
       </c>
-      <c r="F20" t="str">
+      <c r="F22" t="str">
         <v>123456789</v>
       </c>
-      <c r="G20" t="str">
+      <c r="G22" t="str">
         <v>harsh@mai.com</v>
       </c>
-      <c r="H20">
+      <c r="H22" t="str">
         <v>10</v>
       </c>
-      <c r="I20">
+      <c r="I22" t="str">
         <v>9</v>
       </c>
-      <c r="J20" t="str">
+      <c r="J22" t="str">
         <v>wipro</v>
       </c>
-      <c r="K20" t="str">
-        <v>3</v>
-      </c>
-      <c r="L20" t="str">
+      <c r="K22" t="str">
+        <v>3</v>
+      </c>
+      <c r="L22" t="str">
         <v>can_proceed_for_next_level_of_inteview</v>
       </c>
-      <c r="M20" t="str">
+      <c r="M22" t="str">
         <v>shortlisted</v>
       </c>
     </row>

</xml_diff>